<commit_message>
resultados ARIMA diferenciados y tamaño
</commit_message>
<xml_diff>
--- a/codigo_final_organizado/Simulaciones/lineal_NO_estacionario_diferenciado/resultados_2_ESCENARIOS_ARIMA_CON_DIFF.xlsx
+++ b/codigo_final_organizado/Simulaciones/lineal_NO_estacionario_diferenciado/resultados_2_ESCENARIOS_ARIMA_CON_DIFF.xlsx
@@ -536,19 +536,19 @@
         <v>25.77679270376048</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2625177263493114</v>
+        <v>0.2648423062635428</v>
       </c>
       <c r="H2" t="n">
         <v>0.2944259860793316</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3899669040155191</v>
+        <v>0.3999845054128732</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2108556712049222</v>
+        <v>0.1667020416781071</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9885378486184548</v>
+        <v>0.9893093490273974</v>
       </c>
       <c r="L2" t="n">
         <v>0.7735204568118509</v>
@@ -560,7 +560,7 @@
         <v>0.3023253714288707</v>
       </c>
       <c r="O2" t="n">
-        <v>0.2143114962025439</v>
+        <v>0.2314577481323485</v>
       </c>
     </row>
     <row r="3">
@@ -589,31 +589,31 @@
         <v>27.31157121970884</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8137048345559498</v>
+        <v>0.7367725734787592</v>
       </c>
       <c r="H3" t="n">
         <v>0.5362415689082549</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8862691152952242</v>
+        <v>0.8067698848656968</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5374089669908289</v>
+        <v>0.7013610185265239</v>
       </c>
       <c r="K3" t="n">
-        <v>1.079531804581382</v>
+        <v>1.079606318662967</v>
       </c>
       <c r="L3" t="n">
         <v>0.6059360466113632</v>
       </c>
       <c r="M3" t="n">
-        <v>0.49338771618396</v>
+        <v>1.535090727082321</v>
       </c>
       <c r="N3" t="n">
         <v>0.685461050654633</v>
       </c>
       <c r="O3" t="n">
-        <v>0.6933953219620631</v>
+        <v>0.5874117869445946</v>
       </c>
     </row>
     <row r="4">
@@ -642,31 +642,31 @@
         <v>28.12308079889016</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3225790553745564</v>
+        <v>0.3172829080795564</v>
       </c>
       <c r="H4" t="n">
         <v>0.3644925371099176</v>
       </c>
       <c r="I4" t="n">
-        <v>0.4629774148368815</v>
+        <v>0.4556921325965645</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4176243868851081</v>
+        <v>0.2329149865727795</v>
       </c>
       <c r="K4" t="n">
-        <v>1.003046797508251</v>
+        <v>1.006599966677753</v>
       </c>
       <c r="L4" t="n">
         <v>0.2981175496021654</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2626959257833017</v>
+        <v>0.8296464212590471</v>
       </c>
       <c r="N4" t="n">
         <v>0.5860808137790211</v>
       </c>
       <c r="O4" t="n">
-        <v>0.2322457757711952</v>
+        <v>0.3011757366550303</v>
       </c>
     </row>
     <row r="5">
@@ -695,31 +695,31 @@
         <v>26.92358613791478</v>
       </c>
       <c r="G5" t="n">
-        <v>1.01158664024215</v>
+        <v>1.047167857446734</v>
       </c>
       <c r="H5" t="n">
         <v>1.13602931111974</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8508936460387351</v>
+        <v>0.8542726440854786</v>
       </c>
       <c r="J5" t="n">
-        <v>1.60396320850908</v>
+        <v>1.486231553615516</v>
       </c>
       <c r="K5" t="n">
-        <v>0.8500459840964045</v>
+        <v>0.8598011502695897</v>
       </c>
       <c r="L5" t="n">
         <v>1.890531205045505</v>
       </c>
       <c r="M5" t="n">
-        <v>2.066331480047464</v>
+        <v>0.3991767594233399</v>
       </c>
       <c r="N5" t="n">
         <v>1.49183613310364</v>
       </c>
       <c r="O5" t="n">
-        <v>1.472402146149633</v>
+        <v>1.349922214039842</v>
       </c>
     </row>
     <row r="6">
@@ -748,31 +748,31 @@
         <v>25.79666630224374</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9525574174328825</v>
+        <v>0.990122340778822</v>
       </c>
       <c r="H6" t="n">
         <v>2.567193971818427</v>
       </c>
       <c r="I6" t="n">
-        <v>0.7541983563640512</v>
+        <v>0.7849234254131709</v>
       </c>
       <c r="J6" t="n">
-        <v>0.3931727160679734</v>
+        <v>0.491954426243003</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8406811063688824</v>
+        <v>0.8486782587928934</v>
       </c>
       <c r="L6" t="n">
         <v>1.248952593035678</v>
       </c>
       <c r="M6" t="n">
-        <v>1.393675488116779</v>
+        <v>0.3703395202782027</v>
       </c>
       <c r="N6" t="n">
         <v>1.875894935729296</v>
       </c>
       <c r="O6" t="n">
-        <v>0.2067848932960737</v>
+        <v>0.2988408563168703</v>
       </c>
     </row>
     <row r="7">
@@ -801,31 +801,31 @@
         <v>25.43791639263172</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4020277595577636</v>
+        <v>0.4488583611760173</v>
       </c>
       <c r="H7" t="n">
         <v>0.541444406771042</v>
       </c>
       <c r="I7" t="n">
-        <v>0.3569533342188804</v>
+        <v>0.3576788438215815</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2703098523538076</v>
+        <v>0.2735505756474028</v>
       </c>
       <c r="K7" t="n">
-        <v>0.8906589738033739</v>
+        <v>0.8957167478771801</v>
       </c>
       <c r="L7" t="n">
         <v>0.2512816967665725</v>
       </c>
       <c r="M7" t="n">
-        <v>0.2751645067633461</v>
+        <v>0.2605979402896592</v>
       </c>
       <c r="N7" t="n">
         <v>0.1745740303991614</v>
       </c>
       <c r="O7" t="n">
-        <v>0.3990800244342653</v>
+        <v>0.3672874443582904</v>
       </c>
     </row>
     <row r="8">
@@ -854,31 +854,31 @@
         <v>24.40291983537906</v>
       </c>
       <c r="G8" t="n">
-        <v>0.8737193329234112</v>
+        <v>0.9062454332425819</v>
       </c>
       <c r="H8" t="n">
         <v>0.8440177444712131</v>
       </c>
       <c r="I8" t="n">
-        <v>0.72067952927955</v>
+        <v>0.7362623963781584</v>
       </c>
       <c r="J8" t="n">
-        <v>0.3965972396936209</v>
+        <v>0.3023720181096924</v>
       </c>
       <c r="K8" t="n">
-        <v>0.8347535226241747</v>
+        <v>0.8418244561768575</v>
       </c>
       <c r="L8" t="n">
         <v>0.2285845609792513</v>
       </c>
       <c r="M8" t="n">
-        <v>0.2644855082661787</v>
+        <v>0.3392403909474527</v>
       </c>
       <c r="N8" t="n">
         <v>0.7817946431952526</v>
       </c>
       <c r="O8" t="n">
-        <v>0.3520300934399639</v>
+        <v>0.3484605790162927</v>
       </c>
     </row>
     <row r="9">
@@ -907,31 +907,31 @@
         <v>22.96712407901793</v>
       </c>
       <c r="G9" t="n">
-        <v>1.221302280282329</v>
+        <v>1.237113586789377</v>
       </c>
       <c r="H9" t="n">
         <v>0.1580283621872119</v>
       </c>
       <c r="I9" t="n">
-        <v>0.9413212019313514</v>
+        <v>0.9549235379643154</v>
       </c>
       <c r="J9" t="n">
-        <v>0.4114480451613493</v>
+        <v>0.363242646818582</v>
       </c>
       <c r="K9" t="n">
-        <v>0.8287666550490203</v>
+        <v>0.8380172508133381</v>
       </c>
       <c r="L9" t="n">
         <v>0.6549120671590788</v>
       </c>
       <c r="M9" t="n">
-        <v>0.6921152441153984</v>
+        <v>0.5358669738276819</v>
       </c>
       <c r="N9" t="n">
         <v>0.3476930299897104</v>
       </c>
       <c r="O9" t="n">
-        <v>0.4466201660287621</v>
+        <v>0.4564606114509621</v>
       </c>
     </row>
     <row r="10">
@@ -960,31 +960,31 @@
         <v>23.47008885455995</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2257492194867766</v>
+        <v>0.2272709963872031</v>
       </c>
       <c r="H10" t="n">
         <v>2.099676232984059</v>
       </c>
       <c r="I10" t="n">
-        <v>0.3480433069878891</v>
+        <v>0.3505290519841819</v>
       </c>
       <c r="J10" t="n">
-        <v>0.9481074596915887</v>
+        <v>1.105161635716102</v>
       </c>
       <c r="K10" t="n">
-        <v>0.9697381548787531</v>
+        <v>0.9744048986904357</v>
       </c>
       <c r="L10" t="n">
         <v>0.7261019011129686</v>
       </c>
       <c r="M10" t="n">
-        <v>0.6888596560266942</v>
+        <v>0.5866892550215309</v>
       </c>
       <c r="N10" t="n">
         <v>1.612410627313354</v>
       </c>
       <c r="O10" t="n">
-        <v>1.146124265211258</v>
+        <v>0.8871267945290771</v>
       </c>
     </row>
     <row r="11">
@@ -1013,31 +1013,31 @@
         <v>21.48748792140033</v>
       </c>
       <c r="G11" t="n">
-        <v>1.744986768244521</v>
+        <v>1.740248933809657</v>
       </c>
       <c r="H11" t="n">
         <v>1.996854802546846</v>
       </c>
       <c r="I11" t="n">
-        <v>1.484429351788485</v>
+        <v>1.472665161823985</v>
       </c>
       <c r="J11" t="n">
-        <v>1.585849887824712</v>
+        <v>1.470261269805833</v>
       </c>
       <c r="K11" t="n">
-        <v>0.9176385355908128</v>
+        <v>0.9237447867456334</v>
       </c>
       <c r="L11" t="n">
         <v>0.5794622118080914</v>
       </c>
       <c r="M11" t="n">
-        <v>0.5451393203203033</v>
+        <v>1.006566124253472</v>
       </c>
       <c r="N11" t="n">
         <v>1.320844807581292</v>
       </c>
       <c r="O11" t="n">
-        <v>1.566322376313704</v>
+        <v>1.636274910450251</v>
       </c>
     </row>
     <row r="12">
@@ -1066,31 +1066,31 @@
         <v>18.42521173482216</v>
       </c>
       <c r="G12" t="n">
-        <v>2.824873719333177</v>
+        <v>2.808236504563006</v>
       </c>
       <c r="H12" t="n">
         <v>0.3200020371851184</v>
       </c>
       <c r="I12" t="n">
-        <v>2.421898148712654</v>
+        <v>2.43911637503443</v>
       </c>
       <c r="J12" t="n">
-        <v>1.483476417347141</v>
+        <v>1.469662336551587</v>
       </c>
       <c r="K12" t="n">
-        <v>1.69953938613396</v>
+        <v>1.707287010441392</v>
       </c>
       <c r="L12" t="n">
         <v>2.784299128821108</v>
       </c>
       <c r="M12" t="n">
-        <v>2.81683859258197</v>
+        <v>2.066582927066592</v>
       </c>
       <c r="N12" t="n">
         <v>0.3215227717134997</v>
       </c>
       <c r="O12" t="n">
-        <v>0.883471072649426</v>
+        <v>1.257223957844785</v>
       </c>
     </row>
     <row r="13">
@@ -1119,31 +1119,31 @@
         <v>15.20591596892681</v>
       </c>
       <c r="G13" t="n">
-        <v>2.978344164103892</v>
+        <v>2.96375479385902</v>
       </c>
       <c r="H13" t="n">
         <v>0.6457117075203092</v>
       </c>
       <c r="I13" t="n">
-        <v>2.503336857601601</v>
+        <v>2.608351823819266</v>
       </c>
       <c r="J13" t="n">
-        <v>1.273852023076138</v>
+        <v>1.036435725319554</v>
       </c>
       <c r="K13" t="n">
-        <v>1.77027360889029</v>
+        <v>1.780065299615569</v>
       </c>
       <c r="L13" t="n">
         <v>1.444362435027515</v>
       </c>
       <c r="M13" t="n">
-        <v>1.333398810855114</v>
+        <v>2.223288467225127</v>
       </c>
       <c r="N13" t="n">
         <v>0.7335392696998366</v>
       </c>
       <c r="O13" t="n">
-        <v>0.9993623390902834</v>
+        <v>0.7801894478578744</v>
       </c>
     </row>
     <row r="14">
@@ -1172,7 +1172,7 @@
         <v>-9.513637903215555</v>
       </c>
       <c r="G14" t="n">
-        <v>0.6488196006494245</v>
+        <v>0.5293721803614317</v>
       </c>
       <c r="H14" t="n">
         <v>1.089261478257023</v>
@@ -1181,10 +1181,10 @@
         <v>0.6131262800779619</v>
       </c>
       <c r="J14" t="n">
-        <v>0.4168852576480732</v>
+        <v>0.3780563917137483</v>
       </c>
       <c r="K14" t="n">
-        <v>0.6674452663128213</v>
+        <v>0.6705288111468155</v>
       </c>
       <c r="L14" t="n">
         <v>1.077271641814574</v>
@@ -1225,7 +1225,7 @@
         <v>-10.33987893437161</v>
       </c>
       <c r="G15" t="n">
-        <v>0.3743867891158886</v>
+        <v>0.3214587559052511</v>
       </c>
       <c r="H15" t="n">
         <v>0.7054238774208559</v>
@@ -1234,16 +1234,16 @@
         <v>0.435059851598284</v>
       </c>
       <c r="J15" t="n">
-        <v>0.3019387900914517</v>
+        <v>0.2620851585266541</v>
       </c>
       <c r="K15" t="n">
-        <v>0.698192440122445</v>
+        <v>0.7011247130273096</v>
       </c>
       <c r="L15" t="n">
         <v>0.3139419184700867</v>
       </c>
       <c r="M15" t="n">
-        <v>0.2950845679269248</v>
+        <v>0.790585644941196</v>
       </c>
       <c r="N15" t="n">
         <v>0.7109241976272364</v>
@@ -1278,7 +1278,7 @@
         <v>-9.678583996826713</v>
       </c>
       <c r="G16" t="n">
-        <v>0.5565377310944708</v>
+        <v>0.6195532464453075</v>
       </c>
       <c r="H16" t="n">
         <v>0.2714153669911938</v>
@@ -1287,16 +1287,16 @@
         <v>0.4808906390437894</v>
       </c>
       <c r="J16" t="n">
-        <v>0.567665897160509</v>
+        <v>0.5750369945155545</v>
       </c>
       <c r="K16" t="n">
-        <v>0.8695332377537439</v>
+        <v>0.8723360262831423</v>
       </c>
       <c r="L16" t="n">
         <v>0.7898101077822367</v>
       </c>
       <c r="M16" t="n">
-        <v>0.8366366700975153</v>
+        <v>0.2882802641105014</v>
       </c>
       <c r="N16" t="n">
         <v>0.3617304689521427</v>
@@ -1331,7 +1331,7 @@
         <v>-9.16664909727341</v>
       </c>
       <c r="G17" t="n">
-        <v>0.4396522494652252</v>
+        <v>0.5044473022233332</v>
       </c>
       <c r="H17" t="n">
         <v>0.5768381365016904</v>
@@ -1340,16 +1340,16 @@
         <v>0.3846693547938943</v>
       </c>
       <c r="J17" t="n">
-        <v>0.2405978035917656</v>
+        <v>0.2202018135256127</v>
       </c>
       <c r="K17" t="n">
-        <v>0.8528617354534537</v>
+        <v>0.8551202753362673</v>
       </c>
       <c r="L17" t="n">
         <v>0.4419844818798694</v>
       </c>
       <c r="M17" t="n">
-        <v>0.4850169099977822</v>
+        <v>0.2677362010018021</v>
       </c>
       <c r="N17" t="n">
         <v>0.3599017664802</v>
@@ -1384,25 +1384,25 @@
         <v>-9.54525269354251</v>
       </c>
       <c r="G18" t="n">
-        <v>0.1665222890806236</v>
+        <v>0.1769659046176615</v>
       </c>
       <c r="H18" t="n">
         <v>0.5067100860836824</v>
       </c>
       <c r="I18" t="n">
-        <v>0.3009217829586796</v>
+        <v>0.2847458844189225</v>
       </c>
       <c r="J18" t="n">
-        <v>0.2742743976971024</v>
+        <v>0.231952375889422</v>
       </c>
       <c r="K18" t="n">
-        <v>0.7512843782426465</v>
+        <v>0.75329983683942</v>
       </c>
       <c r="L18" t="n">
         <v>0.4602198339074136</v>
       </c>
       <c r="M18" t="n">
-        <v>0.4230423861936247</v>
+        <v>0.456913988622148</v>
       </c>
       <c r="N18" t="n">
         <v>0.4933112894450705</v>
@@ -1437,25 +1437,25 @@
         <v>-10.60866950796466</v>
       </c>
       <c r="G19" t="n">
-        <v>0.5642400783898825</v>
+        <v>0.4603100215000683</v>
       </c>
       <c r="H19" t="n">
         <v>0.5460579660217011</v>
       </c>
       <c r="I19" t="n">
-        <v>0.5874617251378247</v>
+        <v>0.5425801482383638</v>
       </c>
       <c r="J19" t="n">
-        <v>0.4961826349572509</v>
+        <v>0.4295909304226662</v>
       </c>
       <c r="K19" t="n">
-        <v>0.6815939228812945</v>
+        <v>0.6833154897163575</v>
       </c>
       <c r="L19" t="n">
         <v>0.5440641750818667</v>
       </c>
       <c r="M19" t="n">
-        <v>0.5304252684885731</v>
+        <v>1.00899767024709</v>
       </c>
       <c r="N19" t="n">
         <v>0.887033125236464</v>
@@ -1490,25 +1490,25 @@
         <v>-11.00898165851836</v>
       </c>
       <c r="G20" t="n">
-        <v>0.169393046507807</v>
+        <v>0.1782568086682427</v>
       </c>
       <c r="H20" t="n">
         <v>0.2517686375108656</v>
       </c>
       <c r="I20" t="n">
-        <v>0.3044428559933141</v>
+        <v>0.2827058914318142</v>
       </c>
       <c r="J20" t="n">
-        <v>0.2829422674128123</v>
+        <v>0.2703431646217884</v>
       </c>
       <c r="K20" t="n">
-        <v>0.7494488423573549</v>
+        <v>0.7512184662674252</v>
       </c>
       <c r="L20" t="n">
         <v>0.2392530768993275</v>
       </c>
       <c r="M20" t="n">
-        <v>0.2116182163766667</v>
+        <v>0.4701996238443251</v>
       </c>
       <c r="N20" t="n">
         <v>0.3794120136946363</v>
@@ -1543,25 +1543,25 @@
         <v>-11.10656357758912</v>
       </c>
       <c r="G21" t="n">
-        <v>0.1605874199743367</v>
+        <v>0.1957384692117254</v>
       </c>
       <c r="H21" t="n">
         <v>0.4001963812143877</v>
       </c>
       <c r="I21" t="n">
-        <v>0.2722306886265576</v>
+        <v>0.2931407093753178</v>
       </c>
       <c r="J21" t="n">
-        <v>0.2494539573422648</v>
+        <v>0.2233767533978894</v>
       </c>
       <c r="K21" t="n">
-        <v>0.7843709849442577</v>
+        <v>0.7861187593041835</v>
       </c>
       <c r="L21" t="n">
         <v>0.3165423965758565</v>
       </c>
       <c r="M21" t="n">
-        <v>0.3434605586210344</v>
+        <v>0.3320203296529319</v>
       </c>
       <c r="N21" t="n">
         <v>0.4566835856787694</v>
@@ -1596,25 +1596,25 @@
         <v>-10.9181669550724</v>
       </c>
       <c r="G22" t="n">
-        <v>0.2421650216064574</v>
+        <v>0.2995617203586911</v>
       </c>
       <c r="H22" t="n">
         <v>0.2810857240361497</v>
       </c>
       <c r="I22" t="n">
-        <v>0.3104428405843178</v>
+        <v>0.3183782736431794</v>
       </c>
       <c r="J22" t="n">
-        <v>0.2731616661424104</v>
+        <v>0.3338913416917921</v>
       </c>
       <c r="K22" t="n">
-        <v>0.8176413141849549</v>
+        <v>0.8194224785569194</v>
       </c>
       <c r="L22" t="n">
         <v>0.2567889596494128</v>
       </c>
       <c r="M22" t="n">
-        <v>0.231757852118833</v>
+        <v>0.2670639643961904</v>
       </c>
       <c r="N22" t="n">
         <v>0.4479458798506923</v>
@@ -1649,25 +1649,25 @@
         <v>-10.72618923023164</v>
       </c>
       <c r="G23" t="n">
-        <v>0.2438667393530661</v>
+        <v>0.3018427706456829</v>
       </c>
       <c r="H23" t="n">
         <v>0.4536502906197868</v>
       </c>
       <c r="I23" t="n">
-        <v>0.305300893455217</v>
+        <v>0.3019466076076006</v>
       </c>
       <c r="J23" t="n">
-        <v>0.2283338629606355</v>
+        <v>0.2303339987425469</v>
       </c>
       <c r="K23" t="n">
-        <v>0.8185744827693582</v>
+        <v>0.8203472329602192</v>
       </c>
       <c r="L23" t="n">
         <v>0.3035615445279609</v>
       </c>
       <c r="M23" t="n">
-        <v>0.3153657576539202</v>
+        <v>0.2666843675498428</v>
       </c>
       <c r="N23" t="n">
         <v>0.4361438816723869</v>
@@ -1702,25 +1702,25 @@
         <v>-12.2001614671585</v>
       </c>
       <c r="G24" t="n">
-        <v>0.9520536461327184</v>
+        <v>0.7859439470026772</v>
       </c>
       <c r="H24" t="n">
         <v>0.5738253109538206</v>
       </c>
       <c r="I24" t="n">
-        <v>0.8649696639320373</v>
+        <v>0.8647302407095083</v>
       </c>
       <c r="J24" t="n">
-        <v>0.7904148318219875</v>
+        <v>0.8053580720500954</v>
       </c>
       <c r="K24" t="n">
-        <v>0.671812289735029</v>
+        <v>0.6725266679115</v>
       </c>
       <c r="L24" t="n">
         <v>0.9882397675023082</v>
       </c>
       <c r="M24" t="n">
-        <v>1.050373358603461</v>
+        <v>1.406119705266911</v>
       </c>
       <c r="N24" t="n">
         <v>0.9893607438832255</v>
@@ -1755,25 +1755,25 @@
         <v>-12.44897834542954</v>
       </c>
       <c r="G25" t="n">
-        <v>0.1508391512802907</v>
+        <v>0.1676900696445014</v>
       </c>
       <c r="H25" t="n">
         <v>0.2511291232124205</v>
       </c>
       <c r="I25" t="n">
-        <v>0.2711393325062955</v>
+        <v>0.2781656602250006</v>
       </c>
       <c r="J25" t="n">
-        <v>0.4437056036561959</v>
+        <v>0.4387373481867253</v>
       </c>
       <c r="K25" t="n">
-        <v>0.7673996669969362</v>
+        <v>0.7693459925171294</v>
       </c>
       <c r="L25" t="n">
         <v>0.2346016176168173</v>
       </c>
       <c r="M25" t="n">
-        <v>0.1730469013557179</v>
+        <v>0.3896174153040006</v>
       </c>
       <c r="N25" t="n">
         <v>0.4943228036595011</v>

</xml_diff>